<commit_message>
Sprawdzenie całości i wykonanie TC_05
</commit_message>
<xml_diff>
--- a/wyniki_programu/TestCases.xlsx
+++ b/wyniki_programu/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\portfolio\Tester manualny - junior\cafe-project\wyniki_programu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B28CDB6-EEFF-4658-B0AD-FFE3AC02D573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1B5997-E07C-4BE1-AECA-F03548BE1158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Priority</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Weryfikacja wieku i sprzedaż alkoholu tylko osobą do tego uprawnionym</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utworzyć użytkownika niepełnoletniego, a następnie spróbować kupić alkohol </t>
   </si>
   <si>
     <t>1. Uruchomić program 
@@ -95,9 +92,6 @@
     <t>Sprawdzenie czy system sprzeda alkohol osobie pełnoletniej</t>
   </si>
   <si>
-    <t xml:space="preserve">Utworzyć użytkownika pełnoletniego, a następnie spróbować kupić alkohol </t>
-  </si>
-  <si>
     <t>1. Uruchomić program 
 2. Wpisać poprawne imię
 3. Wpisać datę urodzenia klienta(np. 2006-09-09, stan na dzień: 16.02.2026)
@@ -117,12 +111,6 @@
     <t>Negative / Functional / Boundary</t>
   </si>
   <si>
-    <t>Wpisać datę urodzenia użytkownika, który jeszcze się nie urodził</t>
-  </si>
-  <si>
-    <t>MEDIUM</t>
-  </si>
-  <si>
     <t>1. Uruchomić program 
 2. Wpisać poprawne imię
 3. Wpisać datę urodzenia klienta, która jest z przyszłości
@@ -160,13 +148,45 @@
     <t>System wyświetla komunikat ostrzegawczy (np. "Nie ma produktu o takim ID!") i nie dodaje nic do koszyka.</t>
   </si>
   <si>
-    <t>Wybrać produkt, którego id nie ma w naszym programie.</t>
-  </si>
-  <si>
     <t>Weryfikacja błędnego wprowadzenia produktu o nieistniejącym ID</t>
   </si>
   <si>
     <t>System wyświetla komunikat ostrzegawczy (np. "Nie ma produktu o takim ID!") i nie dodaje nic do koszyka</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>Weryfikacja błędnie wprowadzonych danych nie będących liczbami naturalnymi(znakiem z klawiatury)</t>
+  </si>
+  <si>
+    <t>1. Wyświetl listę dostępnych produktów (menu). 
+ 2. Zidentyfikuj najwyższe dostępne ID (np. 7). 
+ 3. W polu wyboru ID wpisz wartość o jeden znak nie będący liczbą naturalną.</t>
+  </si>
+  <si>
+    <t>System wyświetla komunikat ostrzegawczy i nie dodaje nic do koszyka.</t>
+  </si>
+  <si>
+    <t>1. Aplikacja jest uruchomiona. 
+ 2. Dostępna jest lista produktów (menu) zawierająca produkty bez ograniczeń wiekowych oraz produkty oznaczone jako (18+).</t>
+  </si>
+  <si>
+    <t>1. Aplikacja jest uruchomiona. 
+ 2. Baza danych produktów zawiera co najmniej jeden produkt z flaga czy_tylko_dla_pelnoletnich=True.</t>
+  </si>
+  <si>
+    <t>1. Aplikacja jest uruchomiona i wyświetla ekran startowy (rejestracja klienta). 
+ 2. System ma dostęp do aktualnej daty systemowej w celu wyliczenia wieku.</t>
+  </si>
+  <si>
+    <t>1. Klient jest zalogowany/zarejestrowany w systemie. 
+ 2. Pole wejściowe ID produktu oczekuje na wprowadzenie danych przez użytkownika.</t>
+  </si>
+  <si>
+    <t>1. Aplikacja jest uruchomiona. 
+ 2. Klient został pomyślnie zarejestrowany i znajduje się na etapie wyboru produktów. 
+ 3. Tester zna zakres dostępnych ID w menu.</t>
   </si>
 </sst>
 </file>
@@ -487,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,7 +562,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -551,106 +571,135 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>17</v>
+      <c r="H6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>